<commit_message>
some more data analysis
</commit_message>
<xml_diff>
--- a/Data Analysis/data analysis (version 1).xlsx
+++ b/Data Analysis/data analysis (version 1).xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="41" uniqueCount="26">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44" uniqueCount="26">
   <si>
     <t>Tester Index</t>
   </si>
@@ -241,6 +241,11 @@
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleMedium4"/>
+  <colors>
+    <mruColors>
+      <color rgb="FFDBDB00"/>
+    </mruColors>
+  </colors>
 </styleSheet>
 </file>
 
@@ -382,11 +387,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:axId val="2092557016"/>
-        <c:axId val="2092559544"/>
+        <c:axId val="2108034360"/>
+        <c:axId val="2109068504"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="2092557016"/>
+        <c:axId val="2108034360"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -395,7 +400,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2092559544"/>
+        <c:crossAx val="2109068504"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -403,7 +408,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="2092559544"/>
+        <c:axId val="2109068504"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -414,14 +419,13 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2092557016"/>
+        <c:crossAx val="2108034360"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
-      <c:layout/>
       <c:overlay val="0"/>
     </c:legend>
     <c:plotVisOnly val="1"/>
@@ -491,11 +495,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:axId val="2139233832"/>
-        <c:axId val="2141337544"/>
+        <c:axId val="2108085096"/>
+        <c:axId val="2108088040"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="2139233832"/>
+        <c:axId val="2108085096"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -504,7 +508,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2141337544"/>
+        <c:crossAx val="2108088040"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -512,7 +516,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="2141337544"/>
+        <c:axId val="2108088040"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -523,14 +527,13 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2139233832"/>
+        <c:crossAx val="2108085096"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
-      <c:layout/>
       <c:overlay val="0"/>
     </c:legend>
     <c:plotVisOnly val="1"/>
@@ -610,11 +613,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:axId val="2139229400"/>
-        <c:axId val="2142039832"/>
+        <c:axId val="2108115448"/>
+        <c:axId val="2108122600"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="2139229400"/>
+        <c:axId val="2108115448"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -641,13 +644,12 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:overlay val="0"/>
         </c:title>
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2142039832"/>
+        <c:crossAx val="2108122600"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -655,7 +657,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="2142039832"/>
+        <c:axId val="2108122600"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -666,14 +668,13 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2139229400"/>
+        <c:crossAx val="2108115448"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:txPr>
         <a:bodyPr/>
@@ -724,7 +725,7 @@
           <c:order val="0"/>
           <c:tx>
             <c:strRef>
-              <c:f>'Survey Data'!$D$31</c:f>
+              <c:f>'Survey Data'!$D$33</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -736,7 +737,7 @@
           <c:invertIfNegative val="0"/>
           <c:val>
             <c:numRef>
-              <c:f>'Survey Data'!$D$32:$D$39</c:f>
+              <c:f>'Survey Data'!$D$34:$D$41</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="8"/>
@@ -773,7 +774,7 @@
           <c:order val="1"/>
           <c:tx>
             <c:strRef>
-              <c:f>'Survey Data'!$E$31</c:f>
+              <c:f>'Survey Data'!$E$33</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -785,7 +786,7 @@
           <c:invertIfNegative val="0"/>
           <c:val>
             <c:numRef>
-              <c:f>'Survey Data'!$E$32:$E$39</c:f>
+              <c:f>'Survey Data'!$E$34:$E$41</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="8"/>
@@ -822,7 +823,7 @@
           <c:order val="2"/>
           <c:tx>
             <c:strRef>
-              <c:f>'Survey Data'!$F$31</c:f>
+              <c:f>'Survey Data'!$F$33</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -834,7 +835,7 @@
           <c:invertIfNegative val="0"/>
           <c:val>
             <c:numRef>
-              <c:f>'Survey Data'!$F$32:$F$39</c:f>
+              <c:f>'Survey Data'!$F$34:$F$41</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="8"/>
@@ -871,7 +872,7 @@
           <c:order val="3"/>
           <c:tx>
             <c:strRef>
-              <c:f>'Survey Data'!$G$31</c:f>
+              <c:f>'Survey Data'!$G$33</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -883,7 +884,7 @@
           <c:invertIfNegative val="0"/>
           <c:val>
             <c:numRef>
-              <c:f>'Survey Data'!$G$32:$G$39</c:f>
+              <c:f>'Survey Data'!$G$34:$G$41</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="8"/>
@@ -920,7 +921,7 @@
           <c:order val="4"/>
           <c:tx>
             <c:strRef>
-              <c:f>'Survey Data'!$H$31</c:f>
+              <c:f>'Survey Data'!$H$33</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -932,7 +933,7 @@
           <c:invertIfNegative val="0"/>
           <c:val>
             <c:numRef>
-              <c:f>'Survey Data'!$H$32:$H$39</c:f>
+              <c:f>'Survey Data'!$H$34:$H$41</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="8"/>
@@ -973,11 +974,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:axId val="2144536904"/>
-        <c:axId val="2144886648"/>
+        <c:axId val="2107395528"/>
+        <c:axId val="2109085320"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="2144536904"/>
+        <c:axId val="2107395528"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1005,7 +1006,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2144886648"/>
+        <c:crossAx val="2109085320"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1013,7 +1014,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="2144886648"/>
+        <c:axId val="2109085320"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1043,7 +1044,200 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2144536904"/>
+        <c:crossAx val="2107395528"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="r"/>
+      <c:layout/>
+      <c:overlay val="0"/>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="1.0" l="0.75" r="0.75" t="1.0" header="0.5" footer="0.5"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart5.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="118"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="18"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:barChart>
+        <c:barDir val="col"/>
+        <c:grouping val="clustered"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:invertIfNegative val="0"/>
+          <c:dPt>
+            <c:idx val="0"/>
+            <c:invertIfNegative val="0"/>
+            <c:bubble3D val="0"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+            </c:spPr>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="1"/>
+            <c:invertIfNegative val="0"/>
+            <c:bubble3D val="0"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent2"/>
+              </a:solidFill>
+            </c:spPr>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="2"/>
+            <c:invertIfNegative val="0"/>
+            <c:bubble3D val="0"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent3"/>
+              </a:solidFill>
+            </c:spPr>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="3"/>
+            <c:invertIfNegative val="0"/>
+            <c:bubble3D val="0"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent4"/>
+              </a:solidFill>
+            </c:spPr>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="4"/>
+            <c:invertIfNegative val="0"/>
+            <c:bubble3D val="0"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:srgbClr val="DBDB00"/>
+              </a:solidFill>
+            </c:spPr>
+          </c:dPt>
+          <c:errBars>
+            <c:errBarType val="both"/>
+            <c:errValType val="stdErr"/>
+            <c:noEndCap val="0"/>
+          </c:errBars>
+          <c:cat>
+            <c:strRef>
+              <c:f>'Survey Data'!$D$33:$H$33</c:f>
+              <c:strCache>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>Overall Helpfulness</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>Time Reduction</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>Helpful Translations</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>Stress Reduction</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>Less OH</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>'Survey Data'!$D$42:$H$42</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>7.75</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>7.875</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>8.25</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>7.75</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>8.125</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:gapWidth val="150"/>
+        <c:axId val="2063073704"/>
+        <c:axId val="2110870056"/>
+      </c:barChart>
+      <c:catAx>
+        <c:axId val="2063073704"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="2110870056"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="2110870056"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+          <c:max val="10.0"/>
+          <c:min val="0.0"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="2063073704"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1210,13 +1404,13 @@
     <xdr:from>
       <xdr:col>10</xdr:col>
       <xdr:colOff>762000</xdr:colOff>
-      <xdr:row>24</xdr:row>
+      <xdr:row>26</xdr:row>
       <xdr:rowOff>88900</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>14</xdr:col>
       <xdr:colOff>330200</xdr:colOff>
-      <xdr:row>52</xdr:row>
+      <xdr:row>54</xdr:row>
       <xdr:rowOff>152400</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
@@ -1240,13 +1434,13 @@
     <xdr:from>
       <xdr:col>0</xdr:col>
       <xdr:colOff>444500</xdr:colOff>
-      <xdr:row>53</xdr:row>
+      <xdr:row>55</xdr:row>
       <xdr:rowOff>177800</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>11</xdr:col>
       <xdr:colOff>3225800</xdr:colOff>
-      <xdr:row>71</xdr:row>
+      <xdr:row>73</xdr:row>
       <xdr:rowOff>12700</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
@@ -1278,6 +1472,36 @@
         </a:prstGeom>
       </xdr:spPr>
     </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>393700</xdr:colOff>
+      <xdr:row>78</xdr:row>
+      <xdr:rowOff>12700</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>1397000</xdr:colOff>
+      <xdr:row>109</xdr:row>
+      <xdr:rowOff>38100</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="6" name="Chart 5"/>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId3"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
     <xdr:clientData/>
   </xdr:twoCellAnchor>
 </xdr:wsDr>
@@ -1763,10 +1987,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B2:M39"/>
+  <dimension ref="A2:M42"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="J19" workbookViewId="0">
-      <selection activeCell="M57" sqref="M57"/>
+    <sheetView tabSelected="1" topLeftCell="A73" workbookViewId="0">
+      <selection activeCell="L82" sqref="L82"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -1775,7 +1999,7 @@
     <col min="13" max="13" width="84.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:13" ht="16">
+    <row r="2" spans="1:13" ht="16">
       <c r="B2" s="3" t="s">
         <v>6</v>
       </c>
@@ -1786,7 +2010,7 @@
       </c>
       <c r="F2" s="3"/>
     </row>
-    <row r="3" spans="2:13" ht="16">
+    <row r="3" spans="1:13" ht="16">
       <c r="B3" s="3">
         <v>8</v>
       </c>
@@ -1797,7 +2021,7 @@
       </c>
       <c r="F3" s="3"/>
     </row>
-    <row r="4" spans="2:13" ht="16">
+    <row r="4" spans="1:13" ht="16">
       <c r="B4" s="3">
         <v>8</v>
       </c>
@@ -1812,7 +2036,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="5" spans="2:13" ht="16">
+    <row r="5" spans="1:13" ht="16">
       <c r="B5" s="3">
         <v>6</v>
       </c>
@@ -1827,7 +2051,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="6" spans="2:13" ht="16">
+    <row r="6" spans="1:13" ht="16">
       <c r="B6" s="3">
         <v>8</v>
       </c>
@@ -1838,7 +2062,7 @@
       </c>
       <c r="F6" s="3"/>
     </row>
-    <row r="7" spans="2:13" ht="16">
+    <row r="7" spans="1:13" ht="16">
       <c r="B7" s="3">
         <v>8</v>
       </c>
@@ -1849,7 +2073,7 @@
       </c>
       <c r="F7" s="3"/>
     </row>
-    <row r="8" spans="2:13" ht="16">
+    <row r="8" spans="1:13" ht="16">
       <c r="B8" s="3">
         <v>6</v>
       </c>
@@ -1860,7 +2084,7 @@
       </c>
       <c r="F8" s="3"/>
     </row>
-    <row r="9" spans="2:13" ht="16">
+    <row r="9" spans="1:13" ht="16">
       <c r="B9" s="3">
         <v>9</v>
       </c>
@@ -1871,7 +2095,7 @@
       </c>
       <c r="F9" s="3"/>
     </row>
-    <row r="10" spans="2:13" ht="16">
+    <row r="10" spans="1:13" ht="16">
       <c r="B10" s="3">
         <v>9</v>
       </c>
@@ -1882,306 +2106,314 @@
       </c>
       <c r="F10" s="3"/>
     </row>
-    <row r="11" spans="2:13" ht="16">
-      <c r="B11" s="3" t="s">
-        <v>12</v>
+    <row r="11" spans="1:13" ht="16">
+      <c r="A11" t="s">
+        <v>3</v>
+      </c>
+      <c r="B11" s="3">
+        <f>AVERAGE(B3:B10)</f>
+        <v>7.75</v>
       </c>
       <c r="C11" s="3"/>
       <c r="D11" s="3"/>
-      <c r="E11" s="3"/>
+      <c r="E11" s="3">
+        <f>AVERAGE(E3:E10)</f>
+        <v>7.875</v>
+      </c>
       <c r="F11" s="3"/>
-      <c r="L11" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="M11" s="3" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="12" spans="2:13" ht="16">
-      <c r="B12" s="3">
-        <v>9</v>
+    </row>
+    <row r="12" spans="1:13" ht="16">
+      <c r="B12" s="3" t="s">
+        <v>12</v>
       </c>
       <c r="C12" s="3"/>
       <c r="D12" s="3"/>
       <c r="E12" s="3"/>
       <c r="F12" s="3"/>
+      <c r="L12" s="3" t="s">
+        <v>6</v>
+      </c>
       <c r="M12" s="3" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="13" spans="2:13" ht="16">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="13" spans="1:13" ht="16">
       <c r="B13" s="3">
-        <v>8</v>
-      </c>
-      <c r="C13" s="3" t="s">
-        <v>13</v>
-      </c>
+        <v>9</v>
+      </c>
+      <c r="C13" s="3"/>
       <c r="D13" s="3"/>
       <c r="E13" s="3"/>
       <c r="F13" s="3"/>
-    </row>
-    <row r="14" spans="2:13" ht="16">
+      <c r="M13" s="3" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="14" spans="1:13" ht="16">
       <c r="B14" s="3">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="C14" s="3" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="D14" s="3"/>
       <c r="E14" s="3"/>
       <c r="F14" s="3"/>
-      <c r="L14" s="3" t="s">
+    </row>
+    <row r="15" spans="1:13" ht="16">
+      <c r="B15" s="3">
         <v>7</v>
       </c>
-      <c r="M14" s="3" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="15" spans="2:13" ht="16">
-      <c r="B15" s="3">
-        <v>9</v>
-      </c>
-      <c r="C15" s="3"/>
+      <c r="C15" s="3" t="s">
+        <v>14</v>
+      </c>
       <c r="D15" s="3"/>
       <c r="E15" s="3"/>
       <c r="F15" s="3"/>
+      <c r="L15" s="3" t="s">
+        <v>7</v>
+      </c>
       <c r="M15" s="3" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="16" spans="2:13" ht="16">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="16" spans="1:13" ht="16">
       <c r="B16" s="3">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="C16" s="3"/>
       <c r="D16" s="3"/>
       <c r="E16" s="3"/>
       <c r="F16" s="3"/>
-    </row>
-    <row r="17" spans="2:13" ht="16">
+      <c r="M16" s="3" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="17" spans="1:13" ht="16">
       <c r="B17" s="3">
-        <v>5</v>
+        <v>10</v>
       </c>
       <c r="C17" s="3"/>
       <c r="D17" s="3"/>
       <c r="E17" s="3"/>
       <c r="F17" s="3"/>
-      <c r="L17" s="3" t="s">
-        <v>15</v>
-      </c>
-      <c r="M17" s="3" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="18" spans="2:13" ht="16">
+    </row>
+    <row r="18" spans="1:13" ht="16">
       <c r="B18" s="3">
-        <v>10</v>
+        <v>5</v>
       </c>
       <c r="C18" s="3"/>
       <c r="D18" s="3"/>
       <c r="E18" s="3"/>
       <c r="F18" s="3"/>
+      <c r="L18" s="3" t="s">
+        <v>15</v>
+      </c>
       <c r="M18" s="3" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="19" spans="2:13" ht="16">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="19" spans="1:13" ht="16">
       <c r="B19" s="3">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="C19" s="3"/>
       <c r="D19" s="3"/>
       <c r="E19" s="3"/>
       <c r="F19" s="3"/>
-    </row>
-    <row r="20" spans="2:13" ht="16">
-      <c r="B20" s="3" t="s">
-        <v>15</v>
+      <c r="M19" s="3" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="20" spans="1:13" ht="16">
+      <c r="B20" s="3">
+        <v>8</v>
       </c>
       <c r="C20" s="3"/>
       <c r="D20" s="3"/>
-      <c r="E20" s="3" t="s">
-        <v>16</v>
-      </c>
+      <c r="E20" s="3"/>
       <c r="F20" s="3"/>
-      <c r="L20" s="3" t="s">
-        <v>16</v>
-      </c>
-      <c r="M20" s="3" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="21" spans="2:13" ht="16">
+    </row>
+    <row r="21" spans="1:13" ht="16">
+      <c r="A21" t="s">
+        <v>3</v>
+      </c>
       <c r="B21" s="3">
-        <v>8</v>
+        <f>AVERAGE(B13:B20)</f>
+        <v>8.25</v>
       </c>
       <c r="C21" s="3"/>
       <c r="D21" s="3"/>
-      <c r="E21" s="3">
-        <v>8</v>
-      </c>
+      <c r="E21" s="3"/>
       <c r="F21" s="3"/>
-      <c r="M21" s="3" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="22" spans="2:13" ht="16">
-      <c r="B22" s="3">
-        <v>9</v>
-      </c>
-      <c r="C22" s="3" t="s">
-        <v>17</v>
-      </c>
+    </row>
+    <row r="22" spans="1:13" ht="16">
+      <c r="B22" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="C22" s="3"/>
       <c r="D22" s="3"/>
-      <c r="E22" s="3">
-        <v>7</v>
-      </c>
-      <c r="F22" s="3" t="s">
+      <c r="E22" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="F22" s="3"/>
+      <c r="L22" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="M22" s="3" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="23" spans="2:13" ht="16">
+    <row r="23" spans="1:13" ht="16">
       <c r="B23" s="3">
         <v>8</v>
       </c>
-      <c r="C23" s="3" t="s">
-        <v>19</v>
-      </c>
+      <c r="C23" s="3"/>
       <c r="D23" s="3"/>
       <c r="E23" s="3">
-        <v>10</v>
-      </c>
-      <c r="F23" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="F23" s="3"/>
+      <c r="M23" s="3" t="s">
         <v>20</v>
       </c>
-      <c r="L23" s="3" t="s">
-        <v>12</v>
-      </c>
-      <c r="M23" s="3" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="24" spans="2:13" ht="16">
+    </row>
+    <row r="24" spans="1:13" ht="16">
       <c r="B24" s="3">
-        <v>8</v>
-      </c>
-      <c r="C24" s="3"/>
+        <v>9</v>
+      </c>
+      <c r="C24" s="3" t="s">
+        <v>17</v>
+      </c>
       <c r="D24" s="3"/>
       <c r="E24" s="3">
-        <v>10</v>
-      </c>
-      <c r="F24" s="3"/>
-      <c r="M24" s="3" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="25" spans="2:13" ht="16">
+        <v>7</v>
+      </c>
+      <c r="F24" s="3" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="25" spans="1:13" ht="16">
       <c r="B25" s="3">
-        <v>7</v>
-      </c>
-      <c r="C25" s="3"/>
+        <v>8</v>
+      </c>
+      <c r="C25" s="3" t="s">
+        <v>19</v>
+      </c>
       <c r="D25" s="3"/>
       <c r="E25" s="3">
-        <v>9</v>
-      </c>
-      <c r="F25" s="3"/>
-    </row>
-    <row r="26" spans="2:13" ht="16">
+        <v>10</v>
+      </c>
+      <c r="F25" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="L25" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="M25" s="3" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="26" spans="1:13" ht="16">
       <c r="B26" s="3">
-        <v>5</v>
+        <v>8</v>
       </c>
       <c r="C26" s="3"/>
       <c r="D26" s="3"/>
       <c r="E26" s="3">
-        <v>6</v>
+        <v>10</v>
       </c>
       <c r="F26" s="3"/>
-    </row>
-    <row r="27" spans="2:13" ht="16">
+      <c r="M26" s="3" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="27" spans="1:13" ht="16">
       <c r="B27" s="3">
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="C27" s="3"/>
       <c r="D27" s="3"/>
       <c r="E27" s="3">
+        <v>9</v>
+      </c>
+      <c r="F27" s="3"/>
+    </row>
+    <row r="28" spans="1:13" ht="16">
+      <c r="B28" s="3">
+        <v>5</v>
+      </c>
+      <c r="C28" s="3"/>
+      <c r="D28" s="3"/>
+      <c r="E28" s="3">
+        <v>6</v>
+      </c>
+      <c r="F28" s="3"/>
+    </row>
+    <row r="29" spans="1:13" ht="16">
+      <c r="B29" s="3">
         <v>10</v>
       </c>
-      <c r="F27" s="3"/>
-    </row>
-    <row r="28" spans="2:13" ht="16">
-      <c r="B28" s="3">
+      <c r="C29" s="3"/>
+      <c r="D29" s="3"/>
+      <c r="E29" s="3">
+        <v>10</v>
+      </c>
+      <c r="F29" s="3"/>
+    </row>
+    <row r="30" spans="1:13" ht="16">
+      <c r="B30" s="3">
         <v>7</v>
       </c>
-      <c r="E28" s="3">
+      <c r="E30" s="3">
         <v>5</v>
       </c>
     </row>
-    <row r="31" spans="2:13">
-      <c r="D31" t="s">
+    <row r="31" spans="1:13">
+      <c r="A31" t="s">
+        <v>3</v>
+      </c>
+      <c r="B31">
+        <f>AVERAGE(B23:B30)</f>
+        <v>7.75</v>
+      </c>
+      <c r="E31">
+        <f>AVERAGE(E23:E30)</f>
+        <v>8.125</v>
+      </c>
+    </row>
+    <row r="33" spans="4:8">
+      <c r="D33" t="s">
         <v>24</v>
       </c>
-      <c r="E31" t="s">
+      <c r="E33" t="s">
         <v>21</v>
       </c>
-      <c r="F31" t="s">
+      <c r="F33" t="s">
         <v>25</v>
       </c>
-      <c r="G31" t="s">
+      <c r="G33" t="s">
         <v>22</v>
       </c>
-      <c r="H31" t="s">
+      <c r="H33" t="s">
         <v>23</v>
-      </c>
-    </row>
-    <row r="32" spans="2:13" ht="16">
-      <c r="D32" s="3">
-        <v>8</v>
-      </c>
-      <c r="E32" s="3">
-        <v>8</v>
-      </c>
-      <c r="F32" s="3">
-        <v>9</v>
-      </c>
-      <c r="G32" s="3">
-        <v>8</v>
-      </c>
-      <c r="H32" s="3">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="33" spans="4:8" ht="16">
-      <c r="D33" s="3">
-        <v>8</v>
-      </c>
-      <c r="E33" s="3">
-        <v>9</v>
-      </c>
-      <c r="F33" s="3">
-        <v>8</v>
-      </c>
-      <c r="G33" s="3">
-        <v>9</v>
-      </c>
-      <c r="H33" s="3">
-        <v>7</v>
       </c>
     </row>
     <row r="34" spans="4:8" ht="16">
       <c r="D34" s="3">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="E34" s="3">
         <v>8</v>
       </c>
       <c r="F34" s="3">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="G34" s="3">
         <v>8</v>
       </c>
       <c r="H34" s="3">
-        <v>10</v>
+        <v>8</v>
       </c>
     </row>
     <row r="35" spans="4:8" ht="16">
@@ -2189,84 +2421,140 @@
         <v>8</v>
       </c>
       <c r="E35" s="3">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="F35" s="3">
+        <v>8</v>
+      </c>
+      <c r="G35" s="3">
         <v>9</v>
       </c>
-      <c r="G35" s="3">
-        <v>8</v>
-      </c>
       <c r="H35" s="3">
-        <v>10</v>
+        <v>7</v>
       </c>
     </row>
     <row r="36" spans="4:8" ht="16">
       <c r="D36" s="3">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="E36" s="3">
+        <v>8</v>
+      </c>
+      <c r="F36" s="3">
         <v>7</v>
       </c>
-      <c r="F36" s="3">
+      <c r="G36" s="3">
+        <v>8</v>
+      </c>
+      <c r="H36" s="3">
         <v>10</v>
-      </c>
-      <c r="G36" s="3">
-        <v>7</v>
-      </c>
-      <c r="H36" s="3">
-        <v>9</v>
       </c>
     </row>
     <row r="37" spans="4:8" ht="16">
       <c r="D37" s="3">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="E37" s="3">
-        <v>5</v>
+        <v>8</v>
       </c>
       <c r="F37" s="3">
-        <v>5</v>
+        <v>9</v>
       </c>
       <c r="G37" s="3">
-        <v>5</v>
+        <v>8</v>
       </c>
       <c r="H37" s="3">
-        <v>6</v>
+        <v>10</v>
       </c>
     </row>
     <row r="38" spans="4:8" ht="16">
       <c r="D38" s="3">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="E38" s="3">
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="F38" s="3">
         <v>10</v>
       </c>
       <c r="G38" s="3">
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="H38" s="3">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="39" spans="4:8" ht="16">
       <c r="D39" s="3">
+        <v>6</v>
+      </c>
+      <c r="E39" s="3">
+        <v>5</v>
+      </c>
+      <c r="F39" s="3">
+        <v>5</v>
+      </c>
+      <c r="G39" s="3">
+        <v>5</v>
+      </c>
+      <c r="H39" s="3">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="40" spans="4:8" ht="16">
+      <c r="D40" s="3">
         <v>9</v>
       </c>
-      <c r="E39" s="3">
-        <v>8</v>
-      </c>
-      <c r="F39" s="3">
-        <v>8</v>
-      </c>
-      <c r="G39" s="3">
+      <c r="E40" s="3">
+        <v>10</v>
+      </c>
+      <c r="F40" s="3">
+        <v>10</v>
+      </c>
+      <c r="G40" s="3">
+        <v>10</v>
+      </c>
+      <c r="H40" s="3">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="41" spans="4:8" ht="16">
+      <c r="D41" s="3">
+        <v>9</v>
+      </c>
+      <c r="E41" s="3">
+        <v>8</v>
+      </c>
+      <c r="F41" s="3">
+        <v>8</v>
+      </c>
+      <c r="G41" s="3">
         <v>7</v>
       </c>
-      <c r="H39" s="3">
+      <c r="H41" s="3">
         <v>5</v>
+      </c>
+    </row>
+    <row r="42" spans="4:8">
+      <c r="D42">
+        <f>AVERAGE(D34:D41)</f>
+        <v>7.75</v>
+      </c>
+      <c r="E42">
+        <f t="shared" ref="E42:H42" si="0">AVERAGE(E34:E41)</f>
+        <v>7.875</v>
+      </c>
+      <c r="F42">
+        <f t="shared" si="0"/>
+        <v>8.25</v>
+      </c>
+      <c r="G42">
+        <f t="shared" si="0"/>
+        <v>7.75</v>
+      </c>
+      <c r="H42">
+        <f t="shared" si="0"/>
+        <v>8.125</v>
       </c>
     </row>
   </sheetData>

</xml_diff>